<commit_message>
Novo Template , PERFIS
#Agora é possivel ver perfil de user, Professor e Turma
#é POSSIVEL INGRESSAR NA TURMA APARTIR DE BOTAO E VER QUE A PESSOA NAO ESTA NA TURMA E QUE ESTA AGUARDAR APROVACAO
#PROXIMOS PASSOS TIME LINE E PESQUISAR POR TURMA
</commit_message>
<xml_diff>
--- a/data/Users/Teacher/romeu/download/3930697a67c119686f8b5066f2b64f54f4040f542486.xlsx
+++ b/data/Users/Teacher/romeu/download/3930697a67c119686f8b5066f2b64f54f4040f542486.xlsx
@@ -455,11 +455,11 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>177388</v>
+        <v>442846</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>pax pax</t>
+          <t>Booststrape filho</t>
         </is>
       </c>
       <c r="D2" t="n">

</xml_diff>